<commit_message>
Pricesheet for Fri 26 Feb 2021 23:49:47 CAT
</commit_message>
<xml_diff>
--- a/xls-daily-price-sheets/26-02-2021.xlsx
+++ b/xls-daily-price-sheets/26-02-2021.xlsx
@@ -175,141 +175,144 @@
     <t>Opening Price</t>
   </si>
   <si>
+    <t>36.0000</t>
+  </si>
+  <si>
+    <t>1.7850</t>
+  </si>
+  <si>
+    <t>6.5412</t>
+  </si>
+  <si>
+    <t>2.3399</t>
+  </si>
+  <si>
+    <t>16.0009</t>
+  </si>
+  <si>
+    <t>6.3147</t>
+  </si>
+  <si>
+    <t>869.9000</t>
+  </si>
+  <si>
+    <t>110.0000</t>
+  </si>
+  <si>
+    <t>10.3170</t>
+  </si>
+  <si>
+    <t>85.0000</t>
+  </si>
+  <si>
+    <t>19.2821</t>
+  </si>
+  <si>
+    <t>46.1169</t>
+  </si>
+  <si>
+    <t>17.1209</t>
+  </si>
+  <si>
+    <t>3.5000</t>
+  </si>
+  <si>
+    <t>27.5041</t>
+  </si>
+  <si>
+    <t>3.0000</t>
+  </si>
+  <si>
+    <t>1.8777</t>
+  </si>
+  <si>
+    <t>15.5000</t>
+  </si>
+  <si>
+    <t>5.6900</t>
+  </si>
+  <si>
+    <t>0.2972</t>
+  </si>
+  <si>
+    <t>0.3105</t>
+  </si>
+  <si>
+    <t>143.9514</t>
+  </si>
+  <si>
+    <t>60.2353</t>
+  </si>
+  <si>
+    <t>27.6000</t>
+  </si>
+  <si>
+    <t>1.1760</t>
+  </si>
+  <si>
+    <t>19.0000</t>
+  </si>
+  <si>
+    <t>0.0748</t>
+  </si>
+  <si>
+    <t>44.4800</t>
+  </si>
+  <si>
+    <t>7.0000</t>
+  </si>
+  <si>
+    <t>266.1000</t>
+  </si>
+  <si>
+    <t>0.9775</t>
+  </si>
+  <si>
+    <t>6.4389</t>
+  </si>
+  <si>
+    <t>16.0233</t>
+  </si>
+  <si>
+    <t>31.7943</t>
+  </si>
+  <si>
+    <t>23.0000</t>
+  </si>
+  <si>
+    <t>1.5975</t>
+  </si>
+  <si>
+    <t>21.0000</t>
+  </si>
+  <si>
+    <t>21.6089</t>
+  </si>
+  <si>
+    <t>20.2171</t>
+  </si>
+  <si>
+    <t>0.5291</t>
+  </si>
+  <si>
+    <t>0.7000</t>
+  </si>
+  <si>
+    <t>43.0000</t>
+  </si>
+  <si>
+    <t>1.5000</t>
+  </si>
+  <si>
+    <t>6.6200</t>
+  </si>
+  <si>
+    <t>0.5630</t>
+  </si>
+  <si>
     <t>40.0000</t>
   </si>
   <si>
-    <t>1.5738</t>
-  </si>
-  <si>
-    <t>6.5686</t>
-  </si>
-  <si>
-    <t>2.3381</t>
-  </si>
-  <si>
-    <t>15.9999</t>
-  </si>
-  <si>
-    <t>6.0081</t>
-  </si>
-  <si>
-    <t>869.9000</t>
-  </si>
-  <si>
-    <t>110.0000</t>
-  </si>
-  <si>
-    <t>10.0782</t>
-  </si>
-  <si>
-    <t>83.0791</t>
-  </si>
-  <si>
-    <t>19.3248</t>
-  </si>
-  <si>
-    <t>44.6643</t>
-  </si>
-  <si>
-    <t>17.1675</t>
-  </si>
-  <si>
-    <t>3.5000</t>
-  </si>
-  <si>
-    <t>27.5000</t>
-  </si>
-  <si>
-    <t>3.0000</t>
-  </si>
-  <si>
-    <t>1.8800</t>
-  </si>
-  <si>
-    <t>14.5455</t>
-  </si>
-  <si>
-    <t>5.7613</t>
-  </si>
-  <si>
-    <t>0.2506</t>
-  </si>
-  <si>
-    <t>0.3105</t>
-  </si>
-  <si>
-    <t>120.3911</t>
-  </si>
-  <si>
-    <t>60.0703</t>
-  </si>
-  <si>
-    <t>27.6000</t>
-  </si>
-  <si>
-    <t>1.3047</t>
-  </si>
-  <si>
-    <t>19.0000</t>
-  </si>
-  <si>
-    <t>0.0749</t>
-  </si>
-  <si>
-    <t>44.3984</t>
-  </si>
-  <si>
-    <t>7.0000</t>
-  </si>
-  <si>
-    <t>266.1000</t>
-  </si>
-  <si>
-    <t>0.8150</t>
-  </si>
-  <si>
-    <t>6.4389</t>
-  </si>
-  <si>
-    <t>14.8620</t>
-  </si>
-  <si>
-    <t>31.5437</t>
-  </si>
-  <si>
-    <t>24.4167</t>
-  </si>
-  <si>
-    <t>1.5573</t>
-  </si>
-  <si>
-    <t>20.0000</t>
-  </si>
-  <si>
-    <t>21.6089</t>
-  </si>
-  <si>
-    <t>19.5840</t>
-  </si>
-  <si>
-    <t>0.5079</t>
-  </si>
-  <si>
-    <t>0.6350</t>
-  </si>
-  <si>
-    <t>43.0000</t>
-  </si>
-  <si>
-    <t>1.3000</t>
-  </si>
-  <si>
-    <t>5.5200</t>
-  </si>
-  <si>
-    <t>0.5608</t>
-  </si>
-  <si>
     <t>0.0002</t>
   </si>
   <si>
@@ -319,229 +322,226 @@
     <t>8.2000</t>
   </si>
   <si>
-    <t>2.1395</t>
+    <t>2.0933</t>
   </si>
   <si>
     <t>Closing Price</t>
   </si>
   <si>
-    <t>36.0000</t>
-  </si>
-  <si>
-    <t>1.7850</t>
-  </si>
-  <si>
-    <t>6.5412</t>
-  </si>
-  <si>
-    <t>2.3399</t>
-  </si>
-  <si>
-    <t>16.0009</t>
-  </si>
-  <si>
-    <t>6.3147</t>
-  </si>
-  <si>
-    <t>10.3170</t>
-  </si>
-  <si>
-    <t>85.0000</t>
-  </si>
-  <si>
-    <t>19.2821</t>
-  </si>
-  <si>
-    <t>46.1169</t>
-  </si>
-  <si>
-    <t>17.1209</t>
-  </si>
-  <si>
-    <t>27.5042</t>
-  </si>
-  <si>
-    <t>1.8777</t>
-  </si>
-  <si>
-    <t>15.5000</t>
-  </si>
-  <si>
-    <t>5.6900</t>
-  </si>
-  <si>
-    <t>0.2972</t>
-  </si>
-  <si>
-    <t>143.9514</t>
-  </si>
-  <si>
-    <t>60.2353</t>
-  </si>
-  <si>
-    <t>1.1760</t>
-  </si>
-  <si>
-    <t>0.0748</t>
-  </si>
-  <si>
-    <t>44.4800</t>
-  </si>
-  <si>
-    <t>0.9775</t>
-  </si>
-  <si>
-    <t>16.0233</t>
-  </si>
-  <si>
-    <t>31.7943</t>
-  </si>
-  <si>
-    <t>23.0000</t>
-  </si>
-  <si>
-    <t>1.5975</t>
-  </si>
-  <si>
-    <t>21.0000</t>
-  </si>
-  <si>
-    <t>20.2171</t>
-  </si>
-  <si>
-    <t>0.5291</t>
-  </si>
-  <si>
-    <t>0.7000</t>
-  </si>
-  <si>
-    <t>1.5000</t>
-  </si>
-  <si>
-    <t>6.6200</t>
-  </si>
-  <si>
-    <t>0.5630</t>
-  </si>
-  <si>
-    <t>2.0933</t>
+    <t>39.2957</t>
+  </si>
+  <si>
+    <t>1.8113</t>
+  </si>
+  <si>
+    <t>6.6866</t>
+  </si>
+  <si>
+    <t>2.2630</t>
+  </si>
+  <si>
+    <t>16.0000</t>
+  </si>
+  <si>
+    <t>6.3927</t>
+  </si>
+  <si>
+    <t>10.6551</t>
+  </si>
+  <si>
+    <t>75.0000</t>
+  </si>
+  <si>
+    <t>19.4000</t>
+  </si>
+  <si>
+    <t>46.4521</t>
+  </si>
+  <si>
+    <t>17.6204</t>
+  </si>
+  <si>
+    <t>27.5500</t>
+  </si>
+  <si>
+    <t>1.8779</t>
+  </si>
+  <si>
+    <t>18.6000</t>
+  </si>
+  <si>
+    <t>5.7000</t>
+  </si>
+  <si>
+    <t>0.3226</t>
+  </si>
+  <si>
+    <t>121.9286</t>
+  </si>
+  <si>
+    <t>60.9982</t>
+  </si>
+  <si>
+    <t>1.3832</t>
+  </si>
+  <si>
+    <t>0.0750</t>
+  </si>
+  <si>
+    <t>45.0035</t>
+  </si>
+  <si>
+    <t>1.1725</t>
+  </si>
+  <si>
+    <t>17.1661</t>
+  </si>
+  <si>
+    <t>34.9067</t>
+  </si>
+  <si>
+    <t>1.5988</t>
+  </si>
+  <si>
+    <t>20.3416</t>
+  </si>
+  <si>
+    <t>0.5300</t>
+  </si>
+  <si>
+    <t>7.9400</t>
+  </si>
+  <si>
+    <t>0.5744</t>
+  </si>
+  <si>
+    <t>1.1202</t>
+  </si>
+  <si>
+    <t>2.0590</t>
   </si>
   <si>
     <t>Total Traded Volume</t>
   </si>
   <si>
+    <t>1400</t>
+  </si>
+  <si>
+    <t>97300</t>
+  </si>
+  <si>
+    <t>6700</t>
+  </si>
+  <si>
+    <t>21300</t>
+  </si>
+  <si>
+    <t>103900</t>
+  </si>
+  <si>
+    <t>53400</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>3100</t>
+  </si>
+  <si>
+    <t>6917200</t>
+  </si>
+  <si>
+    <t>51800</t>
+  </si>
+  <si>
+    <t>23400</t>
+  </si>
+  <si>
+    <t>311500</t>
+  </si>
+  <si>
+    <t>25000</t>
+  </si>
+  <si>
+    <t>5800</t>
+  </si>
+  <si>
+    <t>48000</t>
+  </si>
+  <si>
+    <t>6400</t>
+  </si>
+  <si>
+    <t>710200</t>
+  </si>
+  <si>
+    <t>900</t>
+  </si>
+  <si>
+    <t>1100</t>
+  </si>
+  <si>
+    <t>5300</t>
+  </si>
+  <si>
+    <t>2800</t>
+  </si>
+  <si>
+    <t>388600</t>
+  </si>
+  <si>
+    <t>110700</t>
+  </si>
+  <si>
+    <t>7736000</t>
+  </si>
+  <si>
+    <t>1108100</t>
+  </si>
+  <si>
+    <t>9400</t>
+  </si>
+  <si>
     <t>500</t>
   </si>
   <si>
-    <t>1000</t>
-  </si>
-  <si>
-    <t>1700</t>
-  </si>
-  <si>
-    <t>102100</t>
-  </si>
-  <si>
-    <t>287800</t>
-  </si>
-  <si>
-    <t>24000</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>62500</t>
-  </si>
-  <si>
-    <t>10000</t>
-  </si>
-  <si>
-    <t>79700</t>
-  </si>
-  <si>
-    <t>60200</t>
-  </si>
-  <si>
-    <t>652000</t>
-  </si>
-  <si>
-    <t>12000</t>
-  </si>
-  <si>
-    <t>74700</t>
-  </si>
-  <si>
-    <t>20400</t>
-  </si>
-  <si>
-    <t>836100</t>
-  </si>
-  <si>
-    <t>16400</t>
-  </si>
-  <si>
-    <t>43100</t>
-  </si>
-  <si>
-    <t>28100</t>
-  </si>
-  <si>
-    <t>42500</t>
-  </si>
-  <si>
-    <t>104300</t>
-  </si>
-  <si>
-    <t>49300</t>
-  </si>
-  <si>
-    <t>168500</t>
-  </si>
-  <si>
-    <t>1500</t>
-  </si>
-  <si>
-    <t>7700</t>
-  </si>
-  <si>
-    <t>200</t>
-  </si>
-  <si>
-    <t>193600</t>
-  </si>
-  <si>
-    <t>3500</t>
-  </si>
-  <si>
-    <t>8900</t>
-  </si>
-  <si>
-    <t>30000</t>
-  </si>
-  <si>
-    <t>255200</t>
-  </si>
-  <si>
-    <t>174200</t>
-  </si>
-  <si>
-    <t>54900</t>
-  </si>
-  <si>
-    <t>200000</t>
+    <t>169000</t>
+  </si>
+  <si>
+    <t>37500</t>
+  </si>
+  <si>
+    <t>158800</t>
+  </si>
+  <si>
+    <t>63600</t>
+  </si>
+  <si>
+    <t>4500</t>
+  </si>
+  <si>
+    <t>434200</t>
+  </si>
+  <si>
+    <t>293700</t>
+  </si>
+  <si>
+    <t>300</t>
   </si>
   <si>
     <t>100</t>
   </si>
   <si>
-    <t>299900</t>
-  </si>
-  <si>
-    <t>2500</t>
-  </si>
-  <si>
-    <t>70300</t>
+    <t>60300</t>
+  </si>
+  <si>
+    <t>16100</t>
+  </si>
+  <si>
+    <t>3600</t>
+  </si>
+  <si>
+    <t>596600</t>
   </si>
 </sst>
 </file>
@@ -899,7 +899,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -927,26 +927,54 @@
         <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D2" t="s">
-        <v>137</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D8" t="s">
         <v>138</v>
@@ -954,13 +982,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D9" t="s">
         <v>139</v>
@@ -968,13 +996,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C10" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D10" t="s">
         <v>140</v>
@@ -982,13 +1010,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C11" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D11" t="s">
         <v>141</v>
@@ -996,13 +1024,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>107</v>
+        <v>59</v>
       </c>
       <c r="D12" t="s">
         <v>142</v>
@@ -1010,13 +1038,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C13" t="s">
-        <v>108</v>
+        <v>60</v>
       </c>
       <c r="D13" t="s">
         <v>143</v>
@@ -1024,13 +1052,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="D14" t="s">
         <v>144</v>
@@ -1038,181 +1066,181 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>111</v>
       </c>
       <c r="D15" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C16" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D16" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C18" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C19" t="s">
-        <v>112</v>
+        <v>66</v>
       </c>
       <c r="D19" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C20" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D20" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C21" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C22" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D22" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C23" t="s">
-        <v>68</v>
+        <v>117</v>
       </c>
       <c r="D23" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C24" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D24" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C25" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D25" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C26" t="s">
-        <v>117</v>
+        <v>73</v>
       </c>
       <c r="D26" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C27" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D27" t="s">
         <v>156</v>
@@ -1220,41 +1248,41 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C28" t="s">
-        <v>73</v>
+        <v>121</v>
       </c>
       <c r="D28" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C29" t="s">
-        <v>119</v>
+        <v>76</v>
       </c>
       <c r="D29" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B30" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C30" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D30" t="s">
         <v>158</v>
@@ -1262,27 +1290,27 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C31" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D31" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B32" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C32" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D32" t="s">
         <v>159</v>
@@ -1290,55 +1318,55 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C33" t="s">
-        <v>78</v>
+        <v>124</v>
       </c>
       <c r="D33" t="s">
-        <v>144</v>
+        <v>160</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C34" t="s">
-        <v>122</v>
+        <v>81</v>
       </c>
       <c r="D34" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C35" t="s">
-        <v>123</v>
+        <v>82</v>
       </c>
       <c r="D35" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C36" t="s">
-        <v>81</v>
+        <v>125</v>
       </c>
       <c r="D36" t="s">
         <v>162</v>
@@ -1346,27 +1374,27 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B37" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C37" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D37" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B38" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C38" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D38" t="s">
         <v>163</v>
@@ -1374,267 +1402,239 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C39" t="s">
-        <v>84</v>
+        <v>127</v>
       </c>
       <c r="D39" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B40" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C40" t="s">
-        <v>125</v>
+        <v>87</v>
       </c>
       <c r="D40" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B41" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C41" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D41" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B42" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C42" t="s">
-        <v>127</v>
+        <v>89</v>
       </c>
       <c r="D42" t="s">
-        <v>140</v>
+        <v>167</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B43" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C43" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="D43" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B44" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C44" t="s">
         <v>129</v>
       </c>
       <c r="D44" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B45" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C45" t="s">
-        <v>90</v>
+        <v>130</v>
       </c>
       <c r="D45" t="s">
-        <v>144</v>
+        <v>169</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B46" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C46" t="s">
-        <v>130</v>
+        <v>93</v>
       </c>
       <c r="D46" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B47" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C47" t="s">
-        <v>131</v>
+        <v>94</v>
       </c>
       <c r="D47" t="s">
-        <v>169</v>
+        <v>142</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B48" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C48" t="s">
-        <v>132</v>
+        <v>95</v>
       </c>
       <c r="D48" t="s">
-        <v>170</v>
+        <v>142</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B49" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C49" t="s">
-        <v>94</v>
+        <v>131</v>
       </c>
       <c r="D49" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B50" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C50" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D50" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B51" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C51" t="s">
-        <v>134</v>
+        <v>98</v>
       </c>
       <c r="D51" t="s">
-        <v>172</v>
+        <v>142</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B52" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C52" t="s">
-        <v>135</v>
+        <v>99</v>
       </c>
       <c r="D52" t="s">
-        <v>173</v>
+        <v>142</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B53" t="s">
-        <v>53</v>
+        <v>100</v>
       </c>
       <c r="C53" t="s">
-        <v>53</v>
+        <v>133</v>
       </c>
       <c r="D53" t="s">
-        <v>144</v>
+        <v>173</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B54" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C54" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D54" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B55" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C55" t="s">
-        <v>99</v>
+        <v>134</v>
       </c>
       <c r="D55" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" t="s">
-        <v>50</v>
-      </c>
-      <c r="B56" t="s">
-        <v>100</v>
-      </c>
-      <c r="C56" t="s">
-        <v>100</v>
-      </c>
-      <c r="D56" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" t="s">
-        <v>51</v>
-      </c>
-      <c r="B57" t="s">
-        <v>101</v>
-      </c>
-      <c r="C57" t="s">
-        <v>136</v>
-      </c>
-      <c r="D57" t="s">
         <v>175</v>
       </c>
     </row>

</xml_diff>